<commit_message>
ini perubahan dan perbaikan
</commit_message>
<xml_diff>
--- a/public/files/template-user.xlsx
+++ b/public/files/template-user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B235A5A-C9C5-4F73-85F5-9D13EA842637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E75A32-7F4E-4B3B-B169-8DB1F3A57CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>nama</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>KK-0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   -</t>
   </si>
 </sst>
 </file>
@@ -466,7 +463,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,9 +512,6 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -534,9 +528,6 @@
       </c>
       <c r="E3" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>